<commit_message>
Added performance graphics, original data, and conclusion
</commit_message>
<xml_diff>
--- a/Aggregate Output.xlsx
+++ b/Aggregate Output.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="34">
   <si>
     <t>Sequential</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>* Where speedup = Time_Sequential / Time_Parallel</t>
+  </si>
+  <si>
+    <t>Performance</t>
   </si>
 </sst>
 </file>
@@ -895,11 +898,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2050452752"/>
-        <c:axId val="-2050379456"/>
+        <c:axId val="-2147265888"/>
+        <c:axId val="-2147271888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2050452752"/>
+        <c:axId val="-2147265888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +1000,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2050379456"/>
+        <c:crossAx val="-2147271888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1005,7 +1008,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2050379456"/>
+        <c:axId val="-2147271888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1114,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2050452752"/>
+        <c:crossAx val="-2147265888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1620,11 +1623,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2061411808"/>
-        <c:axId val="-2050434864"/>
+        <c:axId val="-2147308960"/>
+        <c:axId val="-2147314944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2061411808"/>
+        <c:axId val="-2147308960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,7 +1725,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2050434864"/>
+        <c:crossAx val="-2147314944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1730,7 +1733,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2050434864"/>
+        <c:axId val="-2147314944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1840,7 +1843,795 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061411808"/>
+        <c:crossAx val="-2147308960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Parallel</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Linear Equation Solver Performance Analysis</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Small</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$60:$O$66</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1 Process</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Processes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 Processes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 Processes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16 Processes</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32 Processes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64 Processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$60:$P$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.84931506849315</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.172839506172839</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.952380952380952</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.716981132075471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.617977528089888</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.208333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.968503937007874</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Medium</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$60:$O$66</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1 Process</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Processes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 Processes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 Processes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16 Processes</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32 Processes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64 Processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$60:$Q$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.04225352112676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.097560975609756</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.097560975609756</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.672897196261681</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.74712643678161</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.065040650406504</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.666666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$60:$O$66</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1 Process</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Processes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 Processes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 Processes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16 Processes</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32 Processes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64 Processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$60:$R$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.097560975609756</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.024096385542168</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.716981132075471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.747126436781609</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.464285714285713</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.618122977346278</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Huge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$60:$O$66</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1 Process</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Processes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 Processes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8 Processes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16 Processes</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32 Processes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64 Processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$60:$S$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.329113924050633</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.172839506172839</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.672897196261681</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.681818181818181</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.310344827586207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.28310502283105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2145373152"/>
+        <c:axId val="-2145287104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2145373152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Processes</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2145287104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2145287104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Performance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2145373152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2001,6 +2792,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2505,6 +3336,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3064,6 +4398,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3335,10 +4699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S65"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q6" workbookViewId="0">
-      <selection activeCell="AA30" sqref="AA30"/>
+    <sheetView tabSelected="1" topLeftCell="P58" workbookViewId="0">
+      <selection activeCell="AB85" sqref="AB85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4575,19 +5939,19 @@
         <v>24</v>
       </c>
       <c r="P39" s="5">
-        <f>P10/P10</f>
+        <f t="shared" ref="P39:P45" si="0">P10/P10</f>
         <v>1</v>
       </c>
       <c r="Q39" s="2">
-        <f>P10/Q10</f>
+        <f t="shared" ref="Q39:Q45" si="1">P10/Q10</f>
         <v>1.028169014084507</v>
       </c>
       <c r="R39" s="5">
-        <f>P10/R10</f>
+        <f t="shared" ref="R39:R45" si="2">P10/R10</f>
         <v>0.97333333333333327</v>
       </c>
       <c r="S39" s="5">
-        <f>P10/S10</f>
+        <f t="shared" ref="S39:S45" si="3">P10/S10</f>
         <v>0.92405063291139256</v>
       </c>
     </row>
@@ -4640,19 +6004,19 @@
         <v>25</v>
       </c>
       <c r="P40" s="6">
-        <f>P11/P11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q40" s="1">
-        <f>P11/Q11</f>
+        <f t="shared" si="1"/>
         <v>0.98780487804878048</v>
       </c>
       <c r="R40" s="6">
-        <f>P11/R11</f>
+        <f t="shared" si="2"/>
         <v>0.98780487804878048</v>
       </c>
       <c r="S40" s="6">
-        <f>P11/S11</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -4661,19 +6025,19 @@
         <v>26</v>
       </c>
       <c r="P41" s="6">
-        <f>P12/P12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q41" s="1">
-        <f>P12/Q12</f>
+        <f t="shared" si="1"/>
         <v>1.024390243902439</v>
       </c>
       <c r="R41" s="6">
-        <f>P12/R12</f>
+        <f t="shared" si="2"/>
         <v>1.0120481927710843</v>
       </c>
       <c r="S41" s="6">
-        <f>P12/S12</f>
+        <f t="shared" si="3"/>
         <v>1.05</v>
       </c>
     </row>
@@ -4712,19 +6076,19 @@
         <v>27</v>
       </c>
       <c r="P42" s="5">
-        <f>P13/P13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q42" s="1">
-        <f>P13/Q13</f>
+        <f t="shared" si="1"/>
         <v>0.99065420560747663</v>
       </c>
       <c r="R42" s="5">
-        <f>P13/R13</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S42" s="5">
-        <f>P13/S13</f>
+        <f t="shared" si="3"/>
         <v>0.99065420560747663</v>
       </c>
     </row>
@@ -4763,19 +6127,19 @@
         <v>28</v>
       </c>
       <c r="P43" s="6">
-        <f>P14/P14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q43" s="1">
-        <f>P14/Q14</f>
+        <f t="shared" si="1"/>
         <v>1.0229885057471264</v>
       </c>
       <c r="R43" s="6">
-        <f>P14/R14</f>
+        <f t="shared" si="2"/>
         <v>1.0229885057471262</v>
       </c>
       <c r="S43" s="6">
-        <f>P14/S14</f>
+        <f t="shared" si="3"/>
         <v>1.0113636363636362</v>
       </c>
     </row>
@@ -4814,19 +6178,19 @@
         <v>29</v>
       </c>
       <c r="P44" s="6">
-        <f>P15/P15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q44" s="1">
-        <f>P15/Q15</f>
+        <f t="shared" si="1"/>
         <v>0.78048780487804881</v>
       </c>
       <c r="R44" s="6">
-        <f>P15/R15</f>
+        <f t="shared" si="2"/>
         <v>0.85714285714285698</v>
       </c>
       <c r="S44" s="6">
-        <f>P15/S15</f>
+        <f t="shared" si="3"/>
         <v>0.82758620689655182</v>
       </c>
     </row>
@@ -4865,19 +6229,19 @@
         <v>30</v>
       </c>
       <c r="P45" s="5">
-        <f>P16/P16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q45" s="1">
-        <f>P16/Q16</f>
+        <f t="shared" si="1"/>
         <v>0.84666666666666668</v>
       </c>
       <c r="R45" s="5">
-        <f>P16/R16</f>
+        <f t="shared" si="2"/>
         <v>0.82200647249190939</v>
       </c>
       <c r="S45" s="5">
-        <f>P16/S16</f>
+        <f t="shared" si="3"/>
         <v>1.1598173515981736</v>
       </c>
     </row>
@@ -5334,6 +6698,21 @@
       <c r="L59" s="2">
         <v>0.45</v>
       </c>
+      <c r="O59" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P59" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R59" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S59" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="60" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
@@ -5358,6 +6737,25 @@
       <c r="L60" s="1">
         <v>0.35</v>
       </c>
+      <c r="O60" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="P60" s="5">
+        <f>1/P10</f>
+        <v>6.8493150684931496</v>
+      </c>
+      <c r="Q60" s="2">
+        <f>1/Q10</f>
+        <v>7.0422535211267601</v>
+      </c>
+      <c r="R60" s="5">
+        <f>1/R10</f>
+        <v>6.6666666666666661</v>
+      </c>
+      <c r="S60" s="2">
+        <f>1/S10</f>
+        <v>6.3291139240506329</v>
+      </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
@@ -5382,6 +6780,25 @@
       <c r="L61" s="1">
         <v>0.5</v>
       </c>
+      <c r="O61" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P61" s="6">
+        <f>1/P11</f>
+        <v>6.1728395061728394</v>
+      </c>
+      <c r="Q61" s="2">
+        <f t="shared" ref="Q61:S66" si="4">1/Q11</f>
+        <v>6.0975609756097562</v>
+      </c>
+      <c r="R61" s="6">
+        <f>1/R11</f>
+        <v>6.0975609756097562</v>
+      </c>
+      <c r="S61" s="2">
+        <f t="shared" si="4"/>
+        <v>6.1728395061728394</v>
+      </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
@@ -5406,6 +6823,25 @@
       <c r="L62" s="1">
         <v>0.44</v>
       </c>
+      <c r="O62" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P62" s="6">
+        <f>1/P12</f>
+        <v>5.9523809523809517</v>
+      </c>
+      <c r="Q62" s="2">
+        <f t="shared" si="4"/>
+        <v>6.0975609756097562</v>
+      </c>
+      <c r="R62" s="6">
+        <f>1/R12</f>
+        <v>6.0240963855421681</v>
+      </c>
+      <c r="S62" s="2">
+        <f t="shared" si="4"/>
+        <v>6.25</v>
+      </c>
     </row>
     <row r="63" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
@@ -5430,6 +6866,25 @@
       <c r="L63" s="12">
         <v>0.45</v>
       </c>
+      <c r="O63" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P63" s="5">
+        <f>1/P13</f>
+        <v>4.7169811320754711</v>
+      </c>
+      <c r="Q63" s="2">
+        <f t="shared" si="4"/>
+        <v>4.6728971962616814</v>
+      </c>
+      <c r="R63" s="5">
+        <f>1/R13</f>
+        <v>4.7169811320754711</v>
+      </c>
+      <c r="S63" s="2">
+        <f t="shared" si="4"/>
+        <v>4.6728971962616814</v>
+      </c>
     </row>
     <row r="64" spans="1:19" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
@@ -5461,8 +6916,27 @@
       <c r="M64" s="16" t="s">
         <v>18</v>
       </c>
+      <c r="O64" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P64" s="6">
+        <f>1/P14</f>
+        <v>5.617977528089888</v>
+      </c>
+      <c r="Q64" s="2">
+        <f t="shared" si="4"/>
+        <v>5.7471264367816097</v>
+      </c>
+      <c r="R64" s="6">
+        <f>1/R14</f>
+        <v>5.7471264367816088</v>
+      </c>
+      <c r="S64" s="2">
+        <f t="shared" si="4"/>
+        <v>5.6818181818181817</v>
+      </c>
     </row>
-    <row r="65" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
         <v>5</v>
       </c>
@@ -5484,6 +6958,46 @@
       </c>
       <c r="F65" t="s">
         <v>19</v>
+      </c>
+      <c r="O65" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P65" s="6">
+        <f>1/P15</f>
+        <v>5.208333333333333</v>
+      </c>
+      <c r="Q65" s="2">
+        <f t="shared" si="4"/>
+        <v>4.0650406504065044</v>
+      </c>
+      <c r="R65" s="6">
+        <f>1/R15</f>
+        <v>4.4642857142857135</v>
+      </c>
+      <c r="S65" s="2">
+        <f t="shared" si="4"/>
+        <v>4.3103448275862073</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O66" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P66" s="5">
+        <f>1/P16</f>
+        <v>1.9685039370078741</v>
+      </c>
+      <c r="Q66" s="2">
+        <f t="shared" si="4"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="R66" s="5">
+        <f>1/R16</f>
+        <v>1.6181229773462784</v>
+      </c>
+      <c r="S66" s="2">
+        <f t="shared" si="4"/>
+        <v>2.2831050228310503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>